<commit_message>
auto update queens news 2025-09-09T05:42:19Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,386 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 32-02 31st Avenue in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/08/permits-filed-for-32-02-31st-avenue-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed to expand a two-story structure into a five-story residential building at 32-02 31st Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 32nd Street and 33rd Street, the lot is near the 30th Avenue subway station, served by the N and W trains. Jinjie Wu in Galaxy Astoria LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-08-28T10:30:52+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Thu, 28 Aug 2025 10:30:52 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Permits Filed for 159-31 90th Avenue in Jamaica, Queens</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/08/permits-filed-for-159-31-90th-avenue-in-jamaica-queens.html</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a 14-story mixed-use building at 159-31 90th Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located between 161st Street and Parsons Boulevard, the lot is near the Parson Boulevard subway station, served by the E and F trains. Josef Goodman of Haussmann Development LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-08-14T10:30:33+00:00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Thu, 14 Aug 2025 10:30:33 +0000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Permits Filed for 89-53 165th Street in Jamaica, Queens</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/07/permits-filed-for-89-53-165th-street-in-jamaica-queens.html</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a 12-story mixed-use building at 89-53 165th Street in &lt;a href="https://newyorkyimby.com/neighborhoods/Jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located between Jamaica Avenue and 89th Avenue, the lot is near the 169th Street subway station, served by the F train. Ami Weinstock is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-07-18T10:30:24+00:00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Fri, 18 Jul 2025 10:30:24 +0000</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Refinancing Package Secured For 1 Queens Plaza South At 23-10 Queens Plaza South In Long Island City, Queens</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/07/refinancing-package-secured-for-1-queens-plaza-south-at-23-10-queens-plaza-south-in-long-island-city-queens.html</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Natixis Corporate &amp;#38; Investment Banking has provided $158.2 million in floating-rate financing to refinance 1 Queens Plaza South, a 45-story apartment tower at 23-10 Queens Plaza South in &lt;a href="https://newyorkyimby.com/neighborhoods/long-island-city"&gt;Long Island City&lt;/a&gt;, Queens. Designed by SLCE Architects, the 391-unit building, also known as 1 QPS, was developed by Property Markets Group. The property is located between 23rd and 24th Streets.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2025-07-05T11:30:33+00:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Sat, 05 Jul 2025 11:30:33 +0000</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>YIMBY - Long Island City</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Permits Filed for 30-11 12th Street in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/06/permits-filed-for-30-11-12th-street-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a nine-story residential building at 30-11 12th Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 30th Road and 30th Avenue, the lot is near the 30th Avenue subway station, served by the N and W trains. Samuel Teitelbaum of Palm Tree Consulting Inc. is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-06-29T10:30:41+00:00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Sun, 29 Jun 2025 10:30:41 +0000</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Permits Filed for 30-16 23rd Street in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/06/permits-filed-for-30-16-23rd-street-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a five-story residential building at 30-16 23rd Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 30th Road and 30th Avenue, the lot is near the 30th Avenue subway station, served by the N and W trains. Konstantine Drakopoulos of 42-50 21st Street Realty LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-06-22T10:30:29+00:00</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Sun, 22 Jun 2025 10:30:29 +0000</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Permits Filed for 27-16 43rd Avenue in Long Island City, Queens</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/05/permits-filed-for-27-16-43rd-avenue-in-long-island-city-queens.html</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a 15-story mixed-use building at 27-16 43rd Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/long-island-city"&gt;Long Island City&lt;/a&gt;, Queens. Located between Jackson Avenue and Hunter Street, the lot is near the Queens Plaza subway station, served by the E, M, and R trains. Hang Dong Zhang of CH 41 LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2025-05-27T10:30:24+00:00</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Tue, 27 May 2025 10:30:24 +0000</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>YIMBY - Long Island City</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Permits Filed for 35-20 149th Street in Flushing, Queens</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2024/12/permits-filed-for-35-20-149th-street-in-flushing-queens.html</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a nine-story residential building at 35-20 149th Street in &lt;a href="https://newyorkyimby.com/neighborhoods/flushing"&gt;Flushing&lt;/a&gt;, Queens. Located between 35th Avenue and Northern Boulevard, the lot is near the Main Street subway station, served by the 7 train. Sungmi Son of EKKO is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2024-12-01T11:30:54+00:00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Sun, 01 Dec 2024 11:30:54 +0000</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>YIMBY - Flushing</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Permits Filed for 139-45 35th Avenue in Flushing, Queens</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2022/08/permits-filed-for-139-45-35th-avenue-in-flushing-queens.html</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a six-story mixed-use building at 139-45 35th Avenue in &lt;a href="https://newyorkyimby.com/category/flushing"&gt;Flushing&lt;/a&gt;, Queens. Located between Union Street and Parsons Boulevard, the lot is a short walk from the Main Street subway station, serviced by the 7 train. Lin Li is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2022-08-10T10:30:50+00:00</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Wed, 10 Aug 2022 10:30:50 +0000</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>YIMBY - Flushing</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Permits Filed for 38-20 Parsons Boulevard in Flushing, Queens</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2020/11/permits-filed-for-38-20-parsons-boulevard-in-flushing-queens.html</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a seven-story mixed-use building at 38-20 Parsons Boulevard in &lt;a href="https://newyorkyimby.com/category/flushing"&gt;Flushing&lt;/a&gt;, Queens. Located at the intersection of 38th Avenue and Parsons Boulevard, the corner lot is a few blocks east of the Main Street subway station, serviced by the 7 train. Kenneth Liu under the Eastone Parsons Holding LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2020-11-21T11:30:42+00:00</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Sat, 21 Nov 2020 11:30:42 +0000</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>YIMBY - Flushing</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-09-09T15:26:04Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,310 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>City Planning Commission Approves Jamaica Neighborhood Plan In Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/08/city-planning-commission-approves-jamaica-neighborhood-plan-in-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>The New York City Planning Commission has approved the Jamaica Neighborhood Plan, a rezoning initiative aimed at transforming 230 blocks of &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Led by Mayor Eric Adams and the NYC Department of City Planning, the plan is expected to create over 12,000 new homes, including 4,000 permanently affordable units, along with 7,000 new jobs and more than 2 million square feet of commercial and community space. The plan will now advance to the City Council for final review after two years of development with extensive community engagement.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-08-14T11:30:52+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Thu, 14 Aug 2025 11:30:52 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Jamaica</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Permits Filed for 64-23 Austin Street in Rego Park, Queens</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/06/permits-filed-for-64-23-austin-street-in-rego-park-queens.html</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a six-story residential building at 64-23 Austin Street in &lt;a href="https://newyorkyimby.com/neighborhoods/rego-park"&gt;Rego Park&lt;/a&gt;, Queens. Located between 63rd Drive and 64th Road, the lot is near the 63 Drive-Rego Park subway station, served by the M and R trains. Danil Ilyayev is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-06-19T10:30:09+00:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Thu, 19 Jun 2025 10:30:09 +0000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>YIMBY - Rego Park</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Demolition Nears Completion at 54-03, 54-11 Queens Boulevard in Woodside, Queens</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/03/demolition-nears-completion-at-54-03-54-11-queens-boulevard-in-woodside-queens.html</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Demolition is almost done at 54-03 and 54-11 Queens Boulevard in &lt;a href="https://newyorkyimby.com/neighborhoods/woodside"&gt;Woodside&lt;/a&gt;, Queens. The rectangular 12,000-square-foot property is bound by Queens Boulevard to the south, 55th Street to the east, and 54th Street to the west. Santiago Helman of Nostrand Land LLC is listed as the owner and filed demolition permits, in part, due to the instability of both structures.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-03-23T11:30:59+00:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sun, 23 Mar 2025 11:30:59 +0000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>YIMBY - Woodside</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>38-15 Queens Boulevard’s Steel Superstructure Rises in Sunnyside, Queens</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2024/11/38-15-queens-boulevards-steel-superstructure-rises-in-sunnyside-queens.html</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Construction is rising on 38-15 Queens Boulevard, a two-story car dealership in &lt;a href="https://newyorkyimby.com/neighborhoods/sunnyside"&gt;Sunnyside&lt;/a&gt;, Queens. Developed by Auto Group, which purchased the property along with the abutting 38-08 43rd Avenue for $38 million under the DCO QOZB 38-15 QB LLC in early 2023, the structure will cover 0.69 acres and contain an expansive auto showroom and an ajoining service facility. The project is bound by Queens Boulevard to the south and 39th Street to the east.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-11-10T12:30:35+00:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Sun, 10 Nov 2024 12:30:35 +0000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>YIMBY - Sunnyside</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Developers Secure Refinancing for The Yellowstone at 69-65 Yellowstone Boulevard in Forest Hills, Queens</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2024/03/developers-secure-refinancing-for-the-yellowstone-at-69-65-yellowstone-boulevard-in-forest-hills-queens.html</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://newyorkyimby.com/category/slate-property-group"&gt;Slate Property Group&lt;/a&gt;, in collaboration with Grobman Gross Properties, has finalized a $97 million refinancing deal for The Yellowstone, a recently completed 11-story residential building at &lt;a href="https://newyorkyimby.com/category/69-65-yellowstone-boulevard"&gt;69-65 Yellowstone Boulevard&lt;/a&gt; in &lt;a href="https://newyorkyimby.com/neighborhoods/forest-hills"&gt;Forest Hills&lt;/a&gt;, &lt;a href="https://newyorkyimby.com/category/queens"&gt;Queens&lt;/a&gt;. The refinancing, which will be provided by Apollo Global Real Estate Management L.P., will be used to settle the building's existing debts and support its financial structure.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-03-05T12:00:48+00:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Tue, 05 Mar 2024 12:00:48 +0000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>YIMBY - Forest Hills</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RYBAK Development Secures $71M Loan for The Austin Condominiums in Forest Hills, Queens</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2024/01/rybak-development-secures-71m-loan-for-the-austin-condominiums-in-forest-hills-queens.html</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://newyorkyimby.com/category/rybak-development"&gt;RYBAK Development&lt;/a&gt; has successfully secured a $71 million construction loan for The Austin, a new condominium project located at &lt;a href="https://newyorkyimby.com/category/78-29-austin-street"&gt;78-29 Austin Street&lt;/a&gt; in &lt;a href="https://newyorkyimby.com/neighborhoods/forest-hills"&gt;Forest Hills&lt;/a&gt;, &lt;a href="https://newyorkyimby.com/category/queens"&gt;Queens&lt;/a&gt;. &lt;a href="https://newyorkyimby.com/category/jll-capital-markets"&gt;JLL Capital Markets&lt;/a&gt; facilitated the financing for the project from Valley National Bank.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-01-15T12:00:09+00:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Mon, 15 Jan 2024 12:00:09 +0000</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>YIMBY - Forest Hills</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Permits Filed for 48-37 48th Street in Sunnyside, Queens</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2023/07/permits-filed-for-48-37-48th-street-in-sunnyside-queens.html</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a five-story commercial building at 48-37 48th Street in &lt;a href="https://newyorkyimby.com/category/sunnyside"&gt;Sunnyside&lt;/a&gt;, Queens. Located between 48th Avenue and 50th Avenue, the lot is near the 52nd Street subway station, serviced by the 7 train. Denis Iserovich of &lt;a href="https://newyorkyimby.com/category/east-end-capital"&gt;East End Capital&lt;/a&gt; is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023-07-14T10:30:24+00:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Fri, 14 Jul 2023 10:30:24 +0000</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>YIMBY - Sunnyside</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Myrtle Point Rental Tower Tops Out at 3-50 St. Nicholas Avenue in Ridgewood, Queens</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2022/12/myrtle-point-rental-tower-tops-out-at-3-50-st-nicholas-avenue-in-ridgewood-queens.html</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Construction has topped out on Myrtle Point, a 17-story rental tower at &lt;a href="https://newyorkyimby.com/category/3-50-st-nicholas-avenue-2"&gt;3-50 St. Nicholas Avenue&lt;/a&gt; in &lt;a href="https://newyorkyimby.com/neighborhoods/ridgewood"&gt;Ridgewood&lt;/a&gt;, Queens. Designed by&lt;a href="https://newyorkyimby.com/category/s9-architecture-engineering"&gt; S9 Architecture&lt;/a&gt; and developed in collaboration by Arch Companies and &lt;a href="https://newyorkyimby.com/category/ab-capstone"&gt;AB Capstone&lt;/a&gt;, the building will be the tallest residential property in the Ridgewood-&lt;a href="https://newyorkyimby.com/neighborhoods/bushwick"&gt;Bushwick&lt;/a&gt; area and is expected to debut in 2023.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2022-12-05T12:00:04+00:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Mon, 05 Dec 2022 12:00:04 +0000</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>YIMBY - Ridgewood</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-09-09T17:03:39Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,310 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>City Planning Commission Approves Jamaica Neighborhood Plan In Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/08/city-planning-commission-approves-jamaica-neighborhood-plan-in-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>The New York City Planning Commission has approved the Jamaica Neighborhood Plan, a rezoning initiative aimed at transforming 230 blocks of &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Led by Mayor Eric Adams and the NYC Department of City Planning, the plan is expected to create over 12,000 new homes, including 4,000 permanently affordable units, along with 7,000 new jobs and more than 2 million square feet of commercial and community space. The plan will now advance to the City Council for final review after two years of development with extensive community engagement.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-08-14T11:30:52+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Thu, 14 Aug 2025 11:30:52 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Permits Filed for 64-23 Austin Street in Rego Park, Queens</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/06/permits-filed-for-64-23-austin-street-in-rego-park-queens.html</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a six-story residential building at 64-23 Austin Street in &lt;a href="https://newyorkyimby.com/neighborhoods/rego-park"&gt;Rego Park&lt;/a&gt;, Queens. Located between 63rd Drive and 64th Road, the lot is near the 63 Drive-Rego Park subway station, served by the M and R trains. Danil Ilyayev is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-06-19T10:30:09+00:00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Thu, 19 Jun 2025 10:30:09 +0000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>YIMBY - Rego Park</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Demolition Nears Completion at 54-03, 54-11 Queens Boulevard in Woodside, Queens</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/03/demolition-nears-completion-at-54-03-54-11-queens-boulevard-in-woodside-queens.html</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Demolition is almost done at 54-03 and 54-11 Queens Boulevard in &lt;a href="https://newyorkyimby.com/neighborhoods/woodside"&gt;Woodside&lt;/a&gt;, Queens. The rectangular 12,000-square-foot property is bound by Queens Boulevard to the south, 55th Street to the east, and 54th Street to the west. Santiago Helman of Nostrand Land LLC is listed as the owner and filed demolition permits, in part, due to the instability of both structures.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-03-23T11:30:59+00:00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Sun, 23 Mar 2025 11:30:59 +0000</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>YIMBY - Woodside</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>38-15 Queens Boulevard’s Steel Superstructure Rises in Sunnyside, Queens</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2024/11/38-15-queens-boulevards-steel-superstructure-rises-in-sunnyside-queens.html</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Construction is rising on 38-15 Queens Boulevard, a two-story car dealership in &lt;a href="https://newyorkyimby.com/neighborhoods/sunnyside"&gt;Sunnyside&lt;/a&gt;, Queens. Developed by Auto Group, which purchased the property along with the abutting 38-08 43rd Avenue for $38 million under the DCO QOZB 38-15 QB LLC in early 2023, the structure will cover 0.69 acres and contain an expansive auto showroom and an ajoining service facility. The project is bound by Queens Boulevard to the south and 39th Street to the east.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2024-11-10T12:30:35+00:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Sun, 10 Nov 2024 12:30:35 +0000</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>YIMBY - Sunnyside</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Developers Secure Refinancing for The Yellowstone at 69-65 Yellowstone Boulevard in Forest Hills, Queens</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2024/03/developers-secure-refinancing-for-the-yellowstone-at-69-65-yellowstone-boulevard-in-forest-hills-queens.html</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>&lt;a href="https://newyorkyimby.com/category/slate-property-group"&gt;Slate Property Group&lt;/a&gt;, in collaboration with Grobman Gross Properties, has finalized a $97 million refinancing deal for The Yellowstone, a recently completed 11-story residential building at &lt;a href="https://newyorkyimby.com/category/69-65-yellowstone-boulevard"&gt;69-65 Yellowstone Boulevard&lt;/a&gt; in &lt;a href="https://newyorkyimby.com/neighborhoods/forest-hills"&gt;Forest Hills&lt;/a&gt;, &lt;a href="https://newyorkyimby.com/category/queens"&gt;Queens&lt;/a&gt;. The refinancing, which will be provided by Apollo Global Real Estate Management L.P., will be used to settle the building's existing debts and support its financial structure.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2024-03-05T12:00:48+00:00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Tue, 05 Mar 2024 12:00:48 +0000</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>YIMBY - Forest Hills</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>RYBAK Development Secures $71M Loan for The Austin Condominiums in Forest Hills, Queens</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2024/01/rybak-development-secures-71m-loan-for-the-austin-condominiums-in-forest-hills-queens.html</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>&lt;a href="https://newyorkyimby.com/category/rybak-development"&gt;RYBAK Development&lt;/a&gt; has successfully secured a $71 million construction loan for The Austin, a new condominium project located at &lt;a href="https://newyorkyimby.com/category/78-29-austin-street"&gt;78-29 Austin Street&lt;/a&gt; in &lt;a href="https://newyorkyimby.com/neighborhoods/forest-hills"&gt;Forest Hills&lt;/a&gt;, &lt;a href="https://newyorkyimby.com/category/queens"&gt;Queens&lt;/a&gt;. &lt;a href="https://newyorkyimby.com/category/jll-capital-markets"&gt;JLL Capital Markets&lt;/a&gt; facilitated the financing for the project from Valley National Bank.</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2024-01-15T12:00:09+00:00</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Mon, 15 Jan 2024 12:00:09 +0000</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>YIMBY - Forest Hills</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Permits Filed for 48-37 48th Street in Sunnyside, Queens</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2023/07/permits-filed-for-48-37-48th-street-in-sunnyside-queens.html</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a five-story commercial building at 48-37 48th Street in &lt;a href="https://newyorkyimby.com/category/sunnyside"&gt;Sunnyside&lt;/a&gt;, Queens. Located between 48th Avenue and 50th Avenue, the lot is near the 52nd Street subway station, serviced by the 7 train. Denis Iserovich of &lt;a href="https://newyorkyimby.com/category/east-end-capital"&gt;East End Capital&lt;/a&gt; is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2023-07-14T10:30:24+00:00</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Fri, 14 Jul 2023 10:30:24 +0000</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>YIMBY - Sunnyside</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Myrtle Point Rental Tower Tops Out at 3-50 St. Nicholas Avenue in Ridgewood, Queens</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2022/12/myrtle-point-rental-tower-tops-out-at-3-50-st-nicholas-avenue-in-ridgewood-queens.html</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Construction has topped out on Myrtle Point, a 17-story rental tower at &lt;a href="https://newyorkyimby.com/category/3-50-st-nicholas-avenue-2"&gt;3-50 St. Nicholas Avenue&lt;/a&gt; in &lt;a href="https://newyorkyimby.com/neighborhoods/ridgewood"&gt;Ridgewood&lt;/a&gt;, Queens. Designed by&lt;a href="https://newyorkyimby.com/category/s9-architecture-engineering"&gt; S9 Architecture&lt;/a&gt; and developed in collaboration by Arch Companies and &lt;a href="https://newyorkyimby.com/category/ab-capstone"&gt;AB Capstone&lt;/a&gt;, the building will be the tallest residential property in the Ridgewood-&lt;a href="https://newyorkyimby.com/neighborhoods/bushwick"&gt;Bushwick&lt;/a&gt; area and is expected to debut in 2023.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2022-12-05T12:00:04+00:00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Mon, 05 Dec 2022 12:00:04 +0000</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>YIMBY - Ridgewood</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-09-14T13:02:53Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,82 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Centric Tops Out at 58-01 Queens Boulevard in Woodside, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/09/centric-tops-out-at-58-01-queens-boulevard-in-woodside-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Construction has topped out on Centric, a 12-story residential building at 58-01 Queens Boulevard in &lt;a href="https://newyorkyimby.com/neighborhoods/woodside"&gt;Woodside&lt;/a&gt;, Queens. Designed by Tang Studio Architect and developed by New Empire Corporation, the structure will yield 131 condominium units in one- to three-bedroom layouts, as well as a collection of townhomes. The property is bounded by 44th Avenue to the north, Queens Boulevard to the south, and 58th Street to the west.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-09-14T11:30:14+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sun, 14 Sep 2025 11:30:14 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Woodside</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>New Permits Filed for 27-05 27th Street in Astoria, Queens</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/09/new-permits-filed-for-27-05-27th-street-in-astoria-queens.html</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>New permits have been filed for a four-story residential building at 27-05 27th Street in &lt;a href="https://newyorkyimby.com/neighborhoods/Astoria"&gt;Astoria&lt;/a&gt;, Queens. Located at the intersection of Newtown Avenue and 27th Street, the lot is three blocks west of the 30th Avenue subway station, served by the N and W trains. Joe D'Amico of Citia Nova, LLC is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-09-14T10:30:36+00:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Sun, 14 Sep 2025 10:30:36 +0000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>YIMBY - Astoria</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-09-15T13:34:45Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,82 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Centric Tops Out at 58-01 Queens Boulevard in Woodside, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/09/centric-tops-out-at-58-01-queens-boulevard-in-woodside-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Construction has topped out on Centric, a 12-story residential building at 58-01 Queens Boulevard in &lt;a href="https://newyorkyimby.com/neighborhoods/woodside"&gt;Woodside&lt;/a&gt;, Queens. Designed by Tang Studio Architect and developed by New Empire Corporation, the structure will yield 131 condominium units in one- to three-bedroom layouts, as well as a collection of townhomes. The property is bounded by 44th Avenue to the north, Queens Boulevard to the south, and 58th Street to the west.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-09-14T11:30:14+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Sun, 14 Sep 2025 11:30:14 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Woodside</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>New Permits Filed for 27-05 27th Street in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/09/new-permits-filed-for-27-05-27th-street-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>New permits have been filed for a four-story residential building at 27-05 27th Street in &lt;a href="https://newyorkyimby.com/neighborhoods/Astoria"&gt;Astoria&lt;/a&gt;, Queens. Located at the intersection of Newtown Avenue and 27th Street, the lot is three blocks west of the 30th Avenue subway station, served by the N and W trains. Joe D'Amico of Citia Nova, LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-09-14T10:30:36+00:00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Sun, 14 Sep 2025 10:30:36 +0000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-01T12:59:04Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 21–69 Shore Boulevard in Astoria, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/10/permits-filed-for-21-69-shore-boulevard-in-astoria-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a four-story residential building at 21–69 Shore Boulevard in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 21st Drive and Ditmars Boulevard, the lot is closest to the Astoria–Ditmars Boulevard subway station, served by the N and W trains. Aryeh Assouline of Impact Builders Corp. is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-10-01T10:30:37+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wed, 01 Oct 2025 10:30:37 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Astoria</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-02T12:54:37Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 21–69 Shore Boulevard in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/10/permits-filed-for-21-69-shore-boulevard-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a four-story residential building at 21–69 Shore Boulevard in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 21st Drive and Ditmars Boulevard, the lot is closest to the Astoria–Ditmars Boulevard subway station, served by the N and W trains. Aryeh Assouline of Impact Builders Corp. is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-10-01T10:30:37+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Wed, 01 Oct 2025 10:30:37 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-04T12:50:03Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 141-21 84th Drive in Jamaica, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/10/permits-filed-for-141-21-84th-drive-in-jamaica-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a four-story residential building at 141-21 84th Drive in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located between 85th Road and Burden Crescent, the lot is near the Briarwood subway station, served by the E and F trains. Jacob Ashkenazie is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-10-04T10:30:36+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sat, 04 Oct 2025 10:30:36 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Jamaica</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-05T12:50:44Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 141-21 84th Drive in Jamaica, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/10/permits-filed-for-141-21-84th-drive-in-jamaica-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a four-story residential building at 141-21 84th Drive in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located between 85th Road and Burden Crescent, the lot is near the Briarwood subway station, served by the E and F trains. Jacob Ashkenazie is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-10-04T10:30:36+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Sat, 04 Oct 2025 10:30:36 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-11T12:50:12Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 35-34 41st Street in Astoria, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/10/permits-filed-for-35-34-41st-street-in-astoria-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a 12-story mixed-use building at 35-34 41st Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 35th and 36th Avenues, the lot is near the Steinway Street subway station, served by the E, F, M, and R trains. Stephen Ohnemus of Domain 41st Street Site B LLC is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-10-11T11:00:47+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sat, 11 Oct 2025 11:00:47 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Astoria</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-12T12:51:03Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 35-34 41st Street in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/10/permits-filed-for-35-34-41st-street-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a 12-story mixed-use building at 35-34 41st Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 35th and 36th Avenues, the lot is near the Steinway Street subway station, served by the E, F, M, and R trains. Stephen Ohnemus of Domain 41st Street Site B LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-10-11T11:00:47+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Sat, 11 Oct 2025 11:00:47 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-17T12:57:33Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 25-21 46th Street in Astoria, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/10/permits-filed-for-25-21-46th-street-in-astoria-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a three-story residential building at 25-21 46th Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 25th and 28th Avenues, the lot is near the 46th Street subway station, served by the E, F, M, and R trains. Vincent Maimone of Artistic Design Corp. is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-10-17T10:30:44+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Fri, 17 Oct 2025 10:30:44 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Astoria</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-18T12:51:56Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 25-21 46th Street in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/10/permits-filed-for-25-21-46th-street-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a three-story residential building at 25-21 46th Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 25th and 28th Avenues, the lot is near the 46th Street subway station, served by the E, F, M, and R trains. Vincent Maimone of Artistic Design Corp. is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-10-17T10:30:44+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Fri, 17 Oct 2025 10:30:44 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-29T13:01:09Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 35-17 42nd Street in Astoria, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/10/permits-filed-for-35-17-42nd-street-in-astoria-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a 16-story mixed-use building at 35-17 42nd Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 75th Street and 76th Street, the lot is one block north of the Freeman Street subway station, served by the 2 and 5 trains. Joel Weiss of Heartfelt Townhouse Build is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-10-29T11:00:45+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wed, 29 Oct 2025 11:00:45 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Astoria</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-10-30T12:59:21Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 35-17 42nd Street in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/10/permits-filed-for-35-17-42nd-street-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a 16-story mixed-use building at 35-17 42nd Street in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between 75th Street and 76th Street, the lot is one block north of the Freeman Street subway station, served by the 2 and 5 trains. Joel Weiss of Heartfelt Townhouse Build is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-10-29T11:00:45+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Wed, 29 Oct 2025 11:00:45 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-11-06T13:00:11Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 148–15 Archer Avenue in Jamaica, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/11/permits-filed-for-148-15-archer-avenue-in-jamaica-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a 22-story affordable housing building at 148–15 Archer Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located at the intersection of 149th Street and Archer Avenue, the lot is near the Sutphin Boulevard–Archer Avenue–JFK Airport subway station, served by the E, J, and Z trains. Larry Grubler of Building 163 SC HDFC is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-11-06T11:30:02+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Thu, 06 Nov 2025 11:30:02 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Jamaica</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-11-07T12:58:18Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -478,27 +478,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Permits Filed for 148–15 Archer Avenue in Jamaica, Queens</t>
+          <t>City Council Approves Jamaica Neighborhood Plan In Jamaica, Queens</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://newyorkyimby.com/2025/11/permits-filed-for-148-15-archer-avenue-in-jamaica-queens.html</t>
+          <t>https://newyorkyimby.com/2025/11/city-council-approves-jamaica-neighborhood-plan-in-jamaica-queens.html</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Permits have been filed for a 22-story affordable housing building at 148–15 Archer Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located at the intersection of 149th Street and Archer Avenue, the lot is near the Sutphin Boulevard–Archer Avenue–JFK Airport subway station, served by the E, J, and Z trains. Larry Grubler of Building 163 SC HDFC is listed as the owner behind the applications.</t>
+          <t>The New York City Council has officially approved the Jamaica Neighborhood Plan, a rezoning initiative led by the Department of City Planning under the Adams administration. Spanning nearly 230 blocks in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens, the plan will enable the creation of approximately 12,000 new homes, including 4,000 permanently affordable units, making it the largest Mandatory Inclusionary Housing zone in New York City to date. The plan is also expected to support 7,000 new jobs through over 2 million square feet of new commercial and community facility space.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-11-06T11:30:02+00:00</t>
+          <t>2025-11-07T12:30:41+00:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Thu, 06 Nov 2025 11:30:02 +0000</t>
+          <t>Fri, 07 Nov 2025 12:30:41 +0000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">

</xml_diff>

<commit_message>
auto update queens news 2025-11-08T12:52:45Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>City Council Approves Jamaica Neighborhood Plan In Jamaica, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/11/city-council-approves-jamaica-neighborhood-plan-in-jamaica-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>The New York City Council has officially approved the Jamaica Neighborhood Plan, a rezoning initiative led by the Department of City Planning under the Adams administration. Spanning nearly 230 blocks in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens, the plan will enable the creation of approximately 12,000 new homes, including 4,000 permanently affordable units, making it the largest Mandatory Inclusionary Housing zone in New York City to date. The plan is also expected to support 7,000 new jobs through over 2 million square feet of new commercial and community facility space.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-11-07T12:30:41+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Fri, 07 Nov 2025 12:30:41 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-11-21T12:58:17Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 9-20 Main Avenue in Astoria, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/11/permits-filed-for-9-20-main-avenue-in-astoria-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a six-story mixed-use building at 9-20 Main Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between Welling Court and Vernon Boulevard, the lot is near the Astoria Boulevard subway station, served by the N and W trains. Christina Xiaoping Chang is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-11-21T11:30:03+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Fri, 21 Nov 2025 11:30:03 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Astoria</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-11-22T12:52:18Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 9-20 Main Avenue in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/11/permits-filed-for-9-20-main-avenue-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a six-story mixed-use building at 9-20 Main Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. Located between Welling Court and Vernon Boulevard, the lot is near the Astoria Boulevard subway station, served by the N and W trains. Christina Xiaoping Chang is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-11-21T11:30:03+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Fri, 21 Nov 2025 11:30:03 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-11-25T13:01:39Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>45–40 Vernon Boulevard Tops Out in Long Island City, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/11/45-40-vernon-boulevard-tops-out-in-long-island-city-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Construction has topped out on 45–40 Vernon Boulevard, a 23-story residential building in &lt;a href="https://newyorkyimby.com/neighborhoods/long-island-city"&gt;Long Island City&lt;/a&gt;, Queens. Designed by Archimaera and developed and built by ZD Jasper, the 262-foot-tall structure will span 192,500 square feet and yield 226 units along with lower-level commercial space. The property is located near the intersection of Vernon Boulevard and 46th Avenue.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-11-25T12:30:14+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Tue, 25 Nov 2025 12:30:14 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Long Island City</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-11-26T13:03:03Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>45–40 Vernon Boulevard Tops Out in Long Island City, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/11/45-40-vernon-boulevard-tops-out-in-long-island-city-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Construction has topped out on 45–40 Vernon Boulevard, a 23-story residential building in &lt;a href="https://newyorkyimby.com/neighborhoods/long-island-city"&gt;Long Island City&lt;/a&gt;, Queens. Designed by Archimaera and developed and built by ZD Jasper, the 262-foot-tall structure will span 192,500 square feet and yield 226 units along with lower-level commercial space. The property is located near the intersection of Vernon Boulevard and 46th Avenue.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-11-25T12:30:14+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Tue, 25 Nov 2025 12:30:14 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Long Island City</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-12-16T13:06:31Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 8802 162nd Street in Jamaica, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2025/12/8802-162nd-street-in-jamaica-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for a 14-story mixed-use building at 8802 162nd Street in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located at the intersection of Highland Avenue and 162nd Street, the lot is near the Parsons Boulevard subway station, served by the E and F trains. Sandi Silk of Mural Real Estate Partners is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-12-16T11:30:21+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Tue, 16 Dec 2025 11:30:21 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Jamaica</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2025-12-17T13:05:37Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 8802 162nd Street in Jamaica, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2025/12/8802-162nd-street-in-jamaica-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a 14-story mixed-use building at 8802 162nd Street in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located at the intersection of Highland Avenue and 162nd Street, the lot is near the Parsons Boulevard subway station, served by the E and F trains. Sandi Silk of Mural Real Estate Partners is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-12-16T11:30:21+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Tue, 16 Dec 2025 11:30:21 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-01-11T13:00:46Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Developers Close On $125 Million Loan For 70–28 Grand Central Parkway in Forest Hills, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2026/01/developers-close-on-125-million-loan-for-70-28-grand-central-parkway-in-forest-hills-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Naftali Credit Partners and Madison Realty Capital have closed on a $125 million loan to develop 70–28 Grand Central Parkway, a 13-story residential building in &lt;a href="https://newyorkyimby.com/neighborhoods/forest-hills"&gt;Forest Hills&lt;/a&gt;, Queens. Designed by SLCE Architects, the 252,399-square-foot structure will yield 241 condominium units in studio to three-bedroom layouts. The project will also include a 100-vehicle parking garage and a collection of amenities. The 32,000-square-foot development site is located to the west of Grand Central Parkway between Jewel Avenue and 72nd Road.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-01-10T13:00:24+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sat, 10 Jan 2026 13:00:24 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Forest Hills</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-01-12T13:08:48Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Developers Close On $125 Million Loan For 70–28 Grand Central Parkway in Forest Hills, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2026/01/developers-close-on-125-million-loan-for-70-28-grand-central-parkway-in-forest-hills-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Naftali Credit Partners and Madison Realty Capital have closed on a $125 million loan to develop 70–28 Grand Central Parkway, a 13-story residential building in &lt;a href="https://newyorkyimby.com/neighborhoods/forest-hills"&gt;Forest Hills&lt;/a&gt;, Queens. Designed by SLCE Architects, the 252,399-square-foot structure will yield 241 condominium units in studio to three-bedroom layouts. The project will also include a 100-vehicle parking garage and a collection of amenities. The 32,000-square-foot development site is located to the west of Grand Central Parkway between Jewel Avenue and 72nd Road.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2026-01-10T13:00:24+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Sat, 10 Jan 2026 13:00:24 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Forest Hills</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-01-25T13:02:53Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Construction Progresses on Six Mid-Rise Developments in Astoria, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2026/01/construction-progresses-on-six-mid-rise-developments-in-astoria-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>YIMBY recently photographed the progress of six more mid-rise residential and commercial buildings under construction in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. The projects range from five to 13 stories and are located around the main 31st Street corridor and its elevated subway stations serving the N and W trains.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-01-25T12:30:05+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sun, 25 Jan 2026 12:30:05 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Astoria</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-01-26T13:10:57Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Construction Progresses on Six Mid-Rise Developments in Astoria, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2026/01/construction-progresses-on-six-mid-rise-developments-in-astoria-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>YIMBY recently photographed the progress of six more mid-rise residential and commercial buildings under construction in &lt;a href="https://newyorkyimby.com/neighborhoods/astoria"&gt;Astoria&lt;/a&gt;, Queens. The projects range from five to 13 stories and are located around the main 31st Street corridor and its elevated subway stations serving the N and W trains.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2026-01-25T12:30:05+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Sun, 25 Jan 2026 12:30:05 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Astoria</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-01-28T13:13:07Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Developers Secure $224.3 Million in Bridge Financing for The Italic at 26-32 Jackson Avenue In Long Island City, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2026/01/developers-secure-224-3-million-in-bridge-financing-for-the-italic-at-26-32-jackson-avenue-in-long-island-city-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Developer American Lions has secured $224.3 million in bridge financing for The Italic, a &lt;a href="https://newyorkyimby.com/2025/03/the-italic-completes-construction-at-26-32-jackson-avenue-in-long-island-city-queens.html"&gt;recently completed&lt;/a&gt; residential skyscraper at 26-32 Jackson Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/long-island-city"&gt;Long Island City&lt;/a&gt;, Queens. Designed by SLCE Architects, the 49-story tower yields 363 residential units, including 109 affordable apartments. JLL Capital Markets arranged the financing package for the development team, a joint venture between The Carlyle Group, Fetner Properties, and Lions Group. The property is located at the corner of Jackson Avenue and Purves Street.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-01-28T12:30:04+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wed, 28 Jan 2026 12:30:04 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Long Island City</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-01-29T13:22:15Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -478,27 +478,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Developers Secure $224.3 Million in Bridge Financing for The Italic at 26-32 Jackson Avenue In Long Island City, Queens</t>
+          <t>Permits Filed for 95-28 147th Place in Jamaica, Queens</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://newyorkyimby.com/2026/01/developers-secure-224-3-million-in-bridge-financing-for-the-italic-at-26-32-jackson-avenue-in-long-island-city-queens.html</t>
+          <t>https://newyorkyimby.com/2026/01/permits-filed-for-95-28-147th-place-in-jamaica-queens.html</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Developer American Lions has secured $224.3 million in bridge financing for The Italic, a &lt;a href="https://newyorkyimby.com/2025/03/the-italic-completes-construction-at-26-32-jackson-avenue-in-long-island-city-queens.html"&gt;recently completed&lt;/a&gt; residential skyscraper at 26-32 Jackson Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/long-island-city"&gt;Long Island City&lt;/a&gt;, Queens. Designed by SLCE Architects, the 49-story tower yields 363 residential units, including 109 affordable apartments. JLL Capital Markets arranged the financing package for the development team, a joint venture between The Carlyle Group, Fetner Properties, and Lions Group. The property is located at the corner of Jackson Avenue and Purves Street.</t>
+          <t>Permits have been filed for a 13-story residential building at 95-28 147th Place in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located between 95th Avenue and 97th Avenue, the lot is near the Sutphin Boulevard–Archer Avenue–JFK Airport subway station, served by the E, J, and Z trains. Herman Jacob under East 181st Gardens LLC is listed as the owner behind the applications.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-01-28T12:30:04+00:00</t>
+          <t>2026-01-29T11:30:10+00:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Wed, 28 Jan 2026 12:30:04 +0000</t>
+          <t>Thu, 29 Jan 2026 11:30:10 +0000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>YIMBY - Long Island City</t>
+          <t>YIMBY - Jamaica</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>

</xml_diff>

<commit_message>
auto update queens news 2026-01-30T13:20:24Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 95-28 147th Place in Jamaica, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2026/01/permits-filed-for-95-28-147th-place-in-jamaica-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for a 13-story residential building at 95-28 147th Place in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Located between 95th Avenue and 97th Avenue, the lot is near the Sutphin Boulevard–Archer Avenue–JFK Airport subway station, served by the E, J, and Z trains. Herman Jacob under East 181st Gardens LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2026-01-29T11:30:10+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Thu, 29 Jan 2026 11:30:10 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-02-11T13:47:05Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Permits Filed for 147-02 106th Avenue in Jamaica, Queens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://newyorkyimby.com/2026/02/permits-filed-for-147-02-106th-avenue-in-jamaica-queens.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Permits have been filed for an 11-story residential building at 147-02 106th Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Also addressed as 106-03 Sutphin Boulevard, the corner lot is near the Sutphin Boulevard–Archer Avenue–JFK Airport subway station, served by the E, J, and Z trains. Xue Mei Yi of 12001 Realty LLC is listed as the owner behind the applications.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-02-11T11:30:20+00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wed, 11 Feb 2026 11:30:20 +0000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>YIMBY</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>YIMBY - Jamaica</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
auto update queens news 2026-02-12T13:43:14Z
</commit_message>
<xml_diff>
--- a/data/output/queens_dev_news.xlsx
+++ b/data/output/queens_dev_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,44 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Permits Filed for 147-02 106th Avenue in Jamaica, Queens</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://newyorkyimby.com/2026/02/permits-filed-for-147-02-106th-avenue-in-jamaica-queens.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Permits have been filed for an 11-story residential building at 147-02 106th Avenue in &lt;a href="https://newyorkyimby.com/neighborhoods/jamaica"&gt;Jamaica&lt;/a&gt;, Queens. Also addressed as 106-03 Sutphin Boulevard, the corner lot is near the Sutphin Boulevard–Archer Avenue–JFK Airport subway station, served by the E, J, and Z trains. Xue Mei Yi of 12001 Realty LLC is listed as the owner behind the applications.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2026-02-11T11:30:20+00:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Wed, 11 Feb 2026 11:30:20 +0000</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>YIMBY</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YIMBY - Jamaica</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>